<commit_message>
Update CRONOGRAMA- JOSE MARIA ARGUEDAS - CHUQUI.xlsx
</commit_message>
<xml_diff>
--- a/10.0 CRONOGRAMA/CRONOGRAMA- JOSE MARIA ARGUEDAS - CHUQUI.xlsx
+++ b/10.0 CRONOGRAMA/CRONOGRAMA- JOSE MARIA ARGUEDAS - CHUQUI.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2018\Desktop\TURISMO CASA\IOARR0002-JM-ARGUEDAS\10.0 CRONOGRAMA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepositorioORFEI\IOARR0002-JM-ARGUEDAS\10.0 CRONOGRAMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B8D145-B66C-46D1-93BD-66E9F442702E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FINANCIERO" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">FINANCIERO!$A$1:$F$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">FISICO!$A$1:$R$20</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -173,10 +174,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_-&quot;S/.&quot;* #,##0.00_-;\-&quot;S/.&quot;* #,##0.00_-;_-&quot;S/.&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;S/.&quot;* #,##0.00_-;\-&quot;S/.&quot;* #,##0.00_-;_-&quot;S/.&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -703,34 +704,34 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -749,10 +750,10 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -779,19 +780,19 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -845,22 +846,22 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1813,28 +1814,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="150" zoomScaleNormal="110" zoomScaleSheetLayoutView="150" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="150" zoomScaleNormal="110" zoomScaleSheetLayoutView="150" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="1"/>
+    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
         <v>20</v>
       </c>
@@ -1844,7 +1845,7 @@
       <c r="E1" s="42"/>
       <c r="F1" s="42"/>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
         <v>30</v>
       </c>
@@ -1854,7 +1855,7 @@
       <c r="E2" s="50"/>
       <c r="F2" s="50"/>
     </row>
-    <row r="3" spans="1:6" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
         <v>0</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1889,7 +1890,7 @@
         <v>3477.46</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="46" t="s">
         <v>19</v>
       </c>
@@ -1899,7 +1900,7 @@
       <c r="E5" s="47"/>
       <c r="F5" s="48"/>
     </row>
-    <row r="6" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1914,7 +1915,7 @@
         <v>132332.96</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1932,7 +1933,7 @@
         <v>94758.94</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>15</v>
       </c>
@@ -1947,7 +1948,7 @@
         <v>5024.34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>16</v>
       </c>
@@ -1962,7 +1963,7 @@
         <v>11211.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1977,7 +1978,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1996,23 +1997,25 @@
         <v>249805.19999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="16">
-        <v>9668.3549999999996</v>
+        <f>F12/2</f>
+        <v>31508.89</v>
       </c>
       <c r="D12" s="16">
-        <v>9668.3549999999996</v>
+        <f>F12/2</f>
+        <v>31508.89</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="38">
         <v>63017.78</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
@@ -2030,7 +2033,7 @@
         <v>24961.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>18</v>
       </c>
@@ -2048,7 +2051,7 @@
         <v>15464.06</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2063,7 +2066,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -2078,7 +2081,7 @@
         <v>17290.75</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -2088,11 +2091,11 @@
       </c>
       <c r="C17" s="18">
         <f>SUM(C11:C16)</f>
-        <v>216071.02499999999</v>
+        <v>237911.55999999997</v>
       </c>
       <c r="D17" s="18">
         <f>SUM(D11:D16)</f>
-        <v>93496.444999999992</v>
+        <v>115336.98</v>
       </c>
       <c r="E17" s="18">
         <f>SUM(E11:E16)</f>
@@ -2100,7 +2103,7 @@
       </c>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="43" t="s">
         <v>12</v>
       </c>
@@ -2126,25 +2129,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="150" zoomScaleNormal="110" zoomScaleSheetLayoutView="150" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="150" zoomScaleNormal="110" zoomScaleSheetLayoutView="150" workbookViewId="0">
       <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="1" customWidth="1"/>
-    <col min="2" max="17" width="3.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
+    <col min="2" max="17" width="3.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="46.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="51" t="s">
         <v>32</v>
       </c>
@@ -2166,7 +2169,7 @@
       <c r="Q1" s="52"/>
       <c r="R1" s="52"/>
     </row>
-    <row r="2" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="56" t="s">
         <v>31</v>
       </c>
@@ -2188,7 +2191,7 @@
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
-    <row r="3" spans="1:18" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
         <v>29</v>
       </c>
@@ -2220,7 +2223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="21" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="21" customFormat="1" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="57"/>
       <c r="B4" s="29" t="s">
         <v>21</v>
@@ -2272,7 +2275,7 @@
       </c>
       <c r="R4" s="29"/>
     </row>
-    <row r="5" spans="1:18" s="21" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="21" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>6</v>
       </c>
@@ -2296,7 +2299,7 @@
         <v>3477.46</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="21" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="21" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="53" t="s">
         <v>19</v>
       </c>
@@ -2318,7 +2321,7 @@
       <c r="Q6" s="53"/>
       <c r="R6" s="53"/>
     </row>
-    <row r="7" spans="1:18" s="21" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="21" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>14</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>132332.96</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="21" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" s="21" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>13</v>
       </c>
@@ -2366,7 +2369,7 @@
         <v>94758.94</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="21" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="21" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>15</v>
       </c>
@@ -2390,7 +2393,7 @@
         <v>5024.34</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="21" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="21" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>16</v>
       </c>
@@ -2414,7 +2417,7 @@
         <v>11211.5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="21" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="21" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>17</v>
       </c>
@@ -2438,7 +2441,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="21" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" s="21" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>7</v>
       </c>
@@ -2463,7 +2466,7 @@
         <v>249805.19999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="21" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" s="21" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>8</v>
       </c>
@@ -2487,7 +2490,7 @@
         <v>63017.78</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="21" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" s="21" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>9</v>
       </c>
@@ -2511,7 +2514,7 @@
         <v>24961.5</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="21" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" s="21" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>18</v>
       </c>
@@ -2535,7 +2538,7 @@
         <v>15464.06</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="21" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" s="21" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>10</v>
       </c>
@@ -2559,7 +2562,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="21" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" s="21" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>11</v>
       </c>
@@ -2583,7 +2586,7 @@
         <v>17290.75</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="21" customFormat="1" ht="3.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" s="21" customFormat="1" ht="3.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="64" t="s">
         <v>7</v>
       </c>
@@ -2605,7 +2608,7 @@
       <c r="Q18" s="25"/>
       <c r="R18" s="28"/>
     </row>
-    <row r="19" spans="1:18" s="21" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" s="21" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="65"/>
       <c r="B19" s="58">
         <v>10000</v>
@@ -2633,7 +2636,7 @@
       <c r="Q19" s="63"/>
       <c r="R19" s="32"/>
     </row>
-    <row r="20" spans="1:18" s="21" customFormat="1" ht="13.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" s="21" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="54" t="s">
         <v>12</v>
       </c>

</xml_diff>